<commit_message>
modified code and words
</commit_message>
<xml_diff>
--- a/datas/Data_forecast/predict_Final_Consumption.xlsx
+++ b/datas/Data_forecast/predict_Final_Consumption.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>TRANSPORT</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>AGRICULTURE, FISHING AND MINING</t>
-  </si>
-  <si>
-    <t>CONSTRUCTION AND OTHERS</t>
   </si>
   <si>
     <t>NON-ENERGY CONSUMPTION</t>
@@ -395,13 +392,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,11 +420,8 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>1970</v>
       </c>
@@ -447,16 +441,13 @@
         <v>5.35</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1.46</v>
       </c>
       <c r="H2">
-        <v>1.46</v>
-      </c>
-      <c r="I2">
         <v>58.83</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>1971</v>
       </c>
@@ -476,16 +467,13 @@
         <v>5.32</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1.42</v>
       </c>
       <c r="H3">
-        <v>1.42</v>
-      </c>
-      <c r="I3">
         <v>61.69</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>1972</v>
       </c>
@@ -505,16 +493,13 @@
         <v>5.34</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1.98</v>
       </c>
       <c r="H4">
-        <v>1.98</v>
-      </c>
-      <c r="I4">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>1973</v>
       </c>
@@ -534,16 +519,13 @@
         <v>5.44</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>2.34</v>
       </c>
       <c r="H5">
-        <v>2.34</v>
-      </c>
-      <c r="I5">
         <v>71.69</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>1974</v>
       </c>
@@ -563,16 +545,13 @@
         <v>5.38</v>
       </c>
       <c r="G6">
-        <v>0.01</v>
+        <v>3.26</v>
       </c>
       <c r="H6">
-        <v>3.26</v>
-      </c>
-      <c r="I6">
-        <v>76.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>76.19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>1975</v>
       </c>
@@ -592,16 +571,13 @@
         <v>5.35</v>
       </c>
       <c r="G7">
-        <v>0.02</v>
+        <v>3.39</v>
       </c>
       <c r="H7">
-        <v>3.39</v>
-      </c>
-      <c r="I7">
-        <v>78.48999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>78.47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>1976</v>
       </c>
@@ -621,16 +597,13 @@
         <v>5.43</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>3.68</v>
       </c>
       <c r="H8">
-        <v>3.68</v>
-      </c>
-      <c r="I8">
         <v>83.20999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>1977</v>
       </c>
@@ -650,16 +623,13 @@
         <v>5.5</v>
       </c>
       <c r="G9">
-        <v>0.03</v>
+        <v>3.99</v>
       </c>
       <c r="H9">
-        <v>3.99</v>
-      </c>
-      <c r="I9">
-        <v>85.03</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>1978</v>
       </c>
@@ -679,16 +649,13 @@
         <v>5.37</v>
       </c>
       <c r="G10">
-        <v>0.04</v>
+        <v>5.15</v>
       </c>
       <c r="H10">
-        <v>5.15</v>
-      </c>
-      <c r="I10">
-        <v>88.94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>88.91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>1979</v>
       </c>
@@ -708,16 +675,13 @@
         <v>5.57</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>6.1</v>
       </c>
       <c r="H11">
-        <v>6.1</v>
-      </c>
-      <c r="I11">
         <v>93.78</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>1980</v>
       </c>
@@ -737,16 +701,13 @@
         <v>5.75</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>5.55</v>
       </c>
       <c r="H12">
-        <v>5.55</v>
-      </c>
-      <c r="I12">
         <v>94.53</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:8">
       <c r="A13" s="1">
         <v>1981</v>
       </c>
@@ -766,16 +727,13 @@
         <v>5.72</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>5.22</v>
       </c>
       <c r="H13">
-        <v>5.22</v>
-      </c>
-      <c r="I13">
         <v>91.23</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>1982</v>
       </c>
@@ -795,16 +753,13 @@
         <v>5.77</v>
       </c>
       <c r="G14">
-        <v>0.13</v>
+        <v>6.16</v>
       </c>
       <c r="H14">
-        <v>6.16</v>
-      </c>
-      <c r="I14">
-        <v>92.45999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>92.33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>1983</v>
       </c>
@@ -824,16 +779,13 @@
         <v>5.91</v>
       </c>
       <c r="G15">
-        <v>0.12</v>
+        <v>6.92</v>
       </c>
       <c r="H15">
-        <v>6.92</v>
-      </c>
-      <c r="I15">
-        <v>92.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>92.08</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>1984</v>
       </c>
@@ -853,16 +805,13 @@
         <v>5.74</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>7.33</v>
       </c>
       <c r="H16">
-        <v>7.33</v>
-      </c>
-      <c r="I16">
         <v>95.22</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:8">
       <c r="A17" s="1">
         <v>1985</v>
       </c>
@@ -882,16 +831,13 @@
         <v>6.06</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>8.869999999999999</v>
       </c>
       <c r="H17">
-        <v>8.869999999999999</v>
-      </c>
-      <c r="I17">
         <v>99.63</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:8">
       <c r="A18" s="1">
         <v>1986</v>
       </c>
@@ -911,16 +857,13 @@
         <v>5.95</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>8.869999999999999</v>
       </c>
       <c r="H18">
-        <v>8.869999999999999</v>
-      </c>
-      <c r="I18">
         <v>105.25</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:8">
       <c r="A19" s="1">
         <v>1987</v>
       </c>
@@ -940,16 +883,13 @@
         <v>6.39</v>
       </c>
       <c r="G19">
-        <v>0.1</v>
+        <v>9.34</v>
       </c>
       <c r="H19">
-        <v>9.34</v>
-      </c>
-      <c r="I19">
-        <v>108.81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>108.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="1">
         <v>1988</v>
       </c>
@@ -969,16 +909,13 @@
         <v>6.46</v>
       </c>
       <c r="G20">
-        <v>0.09</v>
+        <v>9.279999999999999</v>
       </c>
       <c r="H20">
-        <v>9.279999999999999</v>
-      </c>
-      <c r="I20">
-        <v>109.76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>109.66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="1">
         <v>1989</v>
       </c>
@@ -998,16 +935,13 @@
         <v>6.53</v>
       </c>
       <c r="G21">
-        <v>0.09</v>
+        <v>9.529999999999999</v>
       </c>
       <c r="H21">
-        <v>9.529999999999999</v>
-      </c>
-      <c r="I21">
-        <v>111.49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>111.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="1">
         <v>1990</v>
       </c>
@@ -1027,16 +961,13 @@
         <v>6.51</v>
       </c>
       <c r="G22">
-        <v>0.31</v>
+        <v>9.93</v>
       </c>
       <c r="H22">
-        <v>9.93</v>
-      </c>
-      <c r="I22">
-        <v>114.35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>114.04</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="1">
         <v>1991</v>
       </c>
@@ -1056,16 +987,13 @@
         <v>6.62</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>9.449999999999999</v>
       </c>
       <c r="H23">
-        <v>9.449999999999999</v>
-      </c>
-      <c r="I23">
         <v>115.48</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:8">
       <c r="A24" s="1">
         <v>1992</v>
       </c>
@@ -1085,16 +1013,13 @@
         <v>6.52</v>
       </c>
       <c r="G24">
-        <v>0.14</v>
+        <v>9.68</v>
       </c>
       <c r="H24">
-        <v>9.68</v>
-      </c>
-      <c r="I24">
-        <v>116.86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>116.71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="1">
         <v>1993</v>
       </c>
@@ -1114,16 +1039,13 @@
         <v>6.88</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>9.98</v>
       </c>
       <c r="H25">
-        <v>9.98</v>
-      </c>
-      <c r="I25">
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:8">
       <c r="A26" s="1">
         <v>1994</v>
       </c>
@@ -1143,16 +1065,13 @@
         <v>7.1</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>11.03</v>
       </c>
       <c r="H26">
-        <v>11.03</v>
-      </c>
-      <c r="I26">
         <v>126.26</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:8">
       <c r="A27" s="1">
         <v>1995</v>
       </c>
@@ -1172,16 +1091,13 @@
         <v>7.51</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>10.7</v>
       </c>
       <c r="H27">
-        <v>10.7</v>
-      </c>
-      <c r="I27">
         <v>131.52</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:8">
       <c r="A28" s="1">
         <v>1996</v>
       </c>
@@ -1201,16 +1117,13 @@
         <v>7.75</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>10.73</v>
       </c>
       <c r="H28">
-        <v>10.73</v>
-      </c>
-      <c r="I28">
         <v>138.21</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:8">
       <c r="A29" s="1">
         <v>1997</v>
       </c>
@@ -1230,16 +1143,13 @@
         <v>7.54</v>
       </c>
       <c r="G29">
-        <v>0.39</v>
+        <v>12.52</v>
       </c>
       <c r="H29">
-        <v>12.52</v>
-      </c>
-      <c r="I29">
-        <v>143.1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>142.71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="1">
         <v>1998</v>
       </c>
@@ -1259,16 +1169,13 @@
         <v>7.31</v>
       </c>
       <c r="G30">
-        <v>0.05</v>
+        <v>13.13</v>
       </c>
       <c r="H30">
-        <v>13.13</v>
-      </c>
-      <c r="I30">
-        <v>147.99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>147.94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="1">
         <v>1999</v>
       </c>
@@ -1288,16 +1195,13 @@
         <v>7.98</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>13.55</v>
       </c>
       <c r="H31">
-        <v>13.55</v>
-      </c>
-      <c r="I31">
         <v>155.22</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:8">
       <c r="A32" s="1">
         <v>2000</v>
       </c>
@@ -1317,16 +1221,13 @@
         <v>7.74</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>14.17</v>
       </c>
       <c r="H32">
-        <v>14.17</v>
-      </c>
-      <c r="I32">
         <v>156.81</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:8">
       <c r="A33" s="1">
         <v>2001</v>
       </c>
@@ -1346,16 +1247,13 @@
         <v>8.16</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>13.43</v>
       </c>
       <c r="H33">
-        <v>13.43</v>
-      </c>
-      <c r="I33">
         <v>156.52</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:8">
       <c r="A34" s="1">
         <v>2002</v>
       </c>
@@ -1375,16 +1273,13 @@
         <v>7.82</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>8.130000000000001</v>
       </c>
       <c r="H34">
-        <v>8.130000000000001</v>
-      </c>
-      <c r="I34">
         <v>159.68</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:8">
       <c r="A35" s="1">
         <v>2003</v>
       </c>
@@ -1404,16 +1299,13 @@
         <v>8.16</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>8.25</v>
       </c>
       <c r="H35">
-        <v>8.25</v>
-      </c>
-      <c r="I35">
         <v>161.36</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:8">
       <c r="A36" s="1">
         <v>2004</v>
       </c>
@@ -1433,16 +1325,13 @@
         <v>10.89</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>8.789999999999999</v>
       </c>
       <c r="H36">
-        <v>8.789999999999999</v>
-      </c>
-      <c r="I36">
         <v>170.3</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:8">
       <c r="A37" s="1">
         <v>2005</v>
       </c>
@@ -1462,16 +1351,13 @@
         <v>11.57</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>8.609999999999999</v>
       </c>
       <c r="H37">
-        <v>8.609999999999999</v>
-      </c>
-      <c r="I37">
         <v>173.11</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:8">
       <c r="A38" s="1">
         <v>2006</v>
       </c>
@@ -1491,16 +1377,13 @@
         <v>11.54</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>9.18</v>
       </c>
       <c r="H38">
-        <v>9.18</v>
-      </c>
-      <c r="I38">
         <v>178.28</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:8">
       <c r="A39" s="1">
         <v>2007</v>
       </c>
@@ -1520,16 +1403,13 @@
         <v>12.38</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>9.19</v>
       </c>
       <c r="H39">
-        <v>9.19</v>
-      </c>
-      <c r="I39">
         <v>189.14</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:8">
       <c r="A40" s="1">
         <v>2008</v>
       </c>
@@ -1549,16 +1429,13 @@
         <v>13.22</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>8.609999999999999</v>
       </c>
       <c r="H40">
-        <v>8.609999999999999</v>
-      </c>
-      <c r="I40">
         <v>195.41</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:8">
       <c r="A41" s="1">
         <v>2009</v>
       </c>
@@ -1578,16 +1455,13 @@
         <v>11.86</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>9.050000000000001</v>
       </c>
       <c r="H41">
-        <v>9.050000000000001</v>
-      </c>
-      <c r="I41">
         <v>190.81</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:8">
       <c r="A42" s="1">
         <v>2010</v>
       </c>
@@ -1607,16 +1481,13 @@
         <v>12.95</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>9.869999999999999</v>
       </c>
       <c r="H42">
-        <v>9.869999999999999</v>
-      </c>
-      <c r="I42">
         <v>207.71</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:8">
       <c r="A43" s="1">
         <v>2011</v>
       </c>
@@ -1636,16 +1507,13 @@
         <v>13.18</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>9.289999999999999</v>
       </c>
       <c r="H43">
-        <v>9.289999999999999</v>
-      </c>
-      <c r="I43">
         <v>214.86</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:8">
       <c r="A44" s="1">
         <v>2012</v>
       </c>
@@ -1665,16 +1533,13 @@
         <v>13.58</v>
       </c>
       <c r="G44">
-        <v>0</v>
+        <v>16.86</v>
       </c>
       <c r="H44">
-        <v>16.86</v>
-      </c>
-      <c r="I44">
         <v>229.77</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:8">
       <c r="A45" s="1">
         <v>2013</v>
       </c>
@@ -1694,16 +1559,13 @@
         <v>13.89</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>16.33</v>
       </c>
       <c r="H45">
-        <v>16.33</v>
-      </c>
-      <c r="I45">
         <v>233.71</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:8">
       <c r="A46" s="1">
         <v>2014</v>
       </c>
@@ -1723,16 +1585,13 @@
         <v>14.55</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>16.01</v>
       </c>
       <c r="H46">
-        <v>16.01</v>
-      </c>
-      <c r="I46">
         <v>237.76</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:8">
       <c r="A47" s="1">
         <v>2015</v>
       </c>
@@ -1752,16 +1611,13 @@
         <v>14.81</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>15.22</v>
       </c>
       <c r="H47">
-        <v>15.22</v>
-      </c>
-      <c r="I47">
         <v>232.54</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:8">
       <c r="A48" s="1">
         <v>2016</v>
       </c>
@@ -1781,16 +1637,13 @@
         <v>13.95</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>14.76</v>
       </c>
       <c r="H48">
-        <v>14.76</v>
-      </c>
-      <c r="I48">
         <v>228.65</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:8">
       <c r="A49" s="1">
         <v>2017</v>
       </c>
@@ -1810,16 +1663,13 @@
         <v>14.95</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>15.03</v>
       </c>
       <c r="H49">
-        <v>15.03</v>
-      </c>
-      <c r="I49">
         <v>233</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:8">
       <c r="A50" s="1">
         <v>2018</v>
       </c>
@@ -1839,16 +1689,13 @@
         <v>15.09</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>14.12</v>
       </c>
       <c r="H50">
-        <v>14.12</v>
-      </c>
-      <c r="I50">
         <v>228.67</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:8">
       <c r="A51" s="1">
         <v>2019</v>
       </c>
@@ -1868,16 +1715,13 @@
         <v>15.12</v>
       </c>
       <c r="G51">
-        <v>0</v>
+        <v>14.24</v>
       </c>
       <c r="H51">
-        <v>14.24</v>
-      </c>
-      <c r="I51">
         <v>230.3</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:8">
       <c r="A52" s="1">
         <v>2020</v>
       </c>
@@ -1897,16 +1741,13 @@
         <v>15.17</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>12.56</v>
       </c>
       <c r="H52">
-        <v>12.56</v>
-      </c>
-      <c r="I52">
         <v>226.96</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:8">
       <c r="A53" s="1">
         <v>2021</v>
       </c>
@@ -1926,16 +1767,13 @@
         <v>15.42</v>
       </c>
       <c r="G53">
-        <v>0</v>
+        <v>13.24</v>
       </c>
       <c r="H53">
-        <v>13.24</v>
-      </c>
-      <c r="I53">
         <v>237.19</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:8">
       <c r="A54" s="1">
         <v>2022</v>
       </c>
@@ -1955,16 +1793,13 @@
         <v>15.62</v>
       </c>
       <c r="G54">
-        <v>0.02</v>
+        <v>13</v>
       </c>
       <c r="H54">
-        <v>13</v>
-      </c>
-      <c r="I54">
-        <v>237.75</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
+        <v>237.73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" s="1">
         <v>2023</v>
       </c>
@@ -1984,16 +1819,13 @@
         <v>15.83</v>
       </c>
       <c r="G55">
-        <v>0.02</v>
+        <v>13.77</v>
       </c>
       <c r="H55">
-        <v>13.77</v>
-      </c>
-      <c r="I55">
-        <v>243.21</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
+        <v>243.2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" s="1">
         <v>2024</v>
       </c>
@@ -2013,16 +1845,13 @@
         <v>15.93</v>
       </c>
       <c r="G56">
-        <v>0.02</v>
+        <v>13.77</v>
       </c>
       <c r="H56">
-        <v>13.77</v>
-      </c>
-      <c r="I56">
-        <v>244.04</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
+        <v>244.02</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" s="1">
         <v>2025</v>
       </c>
@@ -2042,16 +1871,13 @@
         <v>16.13</v>
       </c>
       <c r="G57">
-        <v>0.02</v>
+        <v>14.08</v>
       </c>
       <c r="H57">
-        <v>14.08</v>
-      </c>
-      <c r="I57">
-        <v>249.48</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+        <v>249.46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" s="1">
         <v>2026</v>
       </c>
@@ -2071,16 +1897,13 @@
         <v>16.33</v>
       </c>
       <c r="G58">
-        <v>0.02</v>
+        <v>14.39</v>
       </c>
       <c r="H58">
-        <v>14.39</v>
-      </c>
-      <c r="I58">
-        <v>249.88</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
+        <v>249.85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" s="1">
         <v>2027</v>
       </c>
@@ -2100,16 +1923,13 @@
         <v>16.53</v>
       </c>
       <c r="G59">
-        <v>0.02</v>
+        <v>14.39</v>
       </c>
       <c r="H59">
-        <v>14.39</v>
-      </c>
-      <c r="I59">
-        <v>254.35</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
+        <v>254.33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" s="1">
         <v>2028</v>
       </c>
@@ -2129,16 +1949,13 @@
         <v>16.63</v>
       </c>
       <c r="G60">
-        <v>0.02</v>
+        <v>15</v>
       </c>
       <c r="H60">
-        <v>15</v>
-      </c>
-      <c r="I60">
-        <v>257.87</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
+        <v>257.85</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" s="1">
         <v>2029</v>
       </c>
@@ -2158,16 +1975,13 @@
         <v>16.84</v>
       </c>
       <c r="G61">
-        <v>0.02</v>
+        <v>14.7</v>
       </c>
       <c r="H61">
-        <v>14.7</v>
-      </c>
-      <c r="I61">
-        <v>259.96</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
+        <v>259.93</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" s="1">
         <v>2030</v>
       </c>
@@ -2187,16 +2001,13 @@
         <v>16.94</v>
       </c>
       <c r="G62">
-        <v>0.02</v>
+        <v>15.47</v>
       </c>
       <c r="H62">
-        <v>15.47</v>
-      </c>
-      <c r="I62">
-        <v>263.52</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
+        <v>263.49</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" s="1">
         <v>2031</v>
       </c>
@@ -2216,16 +2027,13 @@
         <v>17.14</v>
       </c>
       <c r="G63">
-        <v>0.02</v>
+        <v>15.31</v>
       </c>
       <c r="H63">
-        <v>15.31</v>
-      </c>
-      <c r="I63">
-        <v>266.53</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
+        <v>266.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" s="1">
         <v>2032</v>
       </c>
@@ -2245,16 +2053,13 @@
         <v>17.24</v>
       </c>
       <c r="G64">
-        <v>0.03</v>
+        <v>15.78</v>
       </c>
       <c r="H64">
-        <v>15.78</v>
-      </c>
-      <c r="I64">
-        <v>269.17</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
+        <v>269.14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" s="1">
         <v>2033</v>
       </c>
@@ -2274,16 +2079,13 @@
         <v>17.44</v>
       </c>
       <c r="G65">
-        <v>0.02</v>
+        <v>15.78</v>
       </c>
       <c r="H65">
-        <v>15.78</v>
-      </c>
-      <c r="I65">
-        <v>272.9</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
+        <v>272.88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" s="1">
         <v>2034</v>
       </c>
@@ -2303,16 +2105,13 @@
         <v>17.54</v>
       </c>
       <c r="G66">
-        <v>0.03</v>
+        <v>16.09</v>
       </c>
       <c r="H66">
-        <v>16.09</v>
-      </c>
-      <c r="I66">
-        <v>275.39</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
+        <v>275.36</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" s="1">
         <v>2035</v>
       </c>
@@ -2332,16 +2131,13 @@
         <v>17.75</v>
       </c>
       <c r="G67">
-        <v>0.03</v>
+        <v>16.39</v>
       </c>
       <c r="H67">
-        <v>16.39</v>
-      </c>
-      <c r="I67">
-        <v>278.01</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+        <v>277.98</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" s="1">
         <v>2036</v>
       </c>
@@ -2361,16 +2157,13 @@
         <v>17.85</v>
       </c>
       <c r="G68">
-        <v>0.03</v>
+        <v>16.55</v>
       </c>
       <c r="H68">
-        <v>16.55</v>
-      </c>
-      <c r="I68">
-        <v>281.07</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+        <v>281.04</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" s="1">
         <v>2037</v>
       </c>
@@ -2390,16 +2183,13 @@
         <v>17.95</v>
       </c>
       <c r="G69">
-        <v>0.03</v>
+        <v>17.01</v>
       </c>
       <c r="H69">
-        <v>17.01</v>
-      </c>
-      <c r="I69">
-        <v>284.44</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
+        <v>284.41</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" s="1">
         <v>2038</v>
       </c>
@@ -2419,16 +2209,13 @@
         <v>18.15</v>
       </c>
       <c r="G70">
-        <v>0.03</v>
+        <v>16.86</v>
       </c>
       <c r="H70">
-        <v>16.86</v>
-      </c>
-      <c r="I70">
-        <v>286.49</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
+        <v>286.47</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71" s="1">
         <v>2039</v>
       </c>
@@ -2448,16 +2235,13 @@
         <v>18.25</v>
       </c>
       <c r="G71">
-        <v>0.03</v>
+        <v>17.48</v>
       </c>
       <c r="H71">
-        <v>17.48</v>
-      </c>
-      <c r="I71">
-        <v>290.02</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
+        <v>289.99</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72" s="1">
         <v>2040</v>
       </c>
@@ -2477,16 +2261,13 @@
         <v>18.35</v>
       </c>
       <c r="G72">
-        <v>0.03</v>
+        <v>17.32</v>
       </c>
       <c r="H72">
-        <v>17.32</v>
-      </c>
-      <c r="I72">
-        <v>292.15</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9">
+        <v>292.13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
       <c r="A73" s="1">
         <v>2041</v>
       </c>
@@ -2506,16 +2287,13 @@
         <v>18.55</v>
       </c>
       <c r="G73">
-        <v>0.03</v>
+        <v>17.78</v>
       </c>
       <c r="H73">
-        <v>17.78</v>
-      </c>
-      <c r="I73">
-        <v>295.54</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
+        <v>295.52</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
       <c r="A74" s="1">
         <v>2042</v>
       </c>
@@ -2535,13 +2313,10 @@
         <v>18.66</v>
       </c>
       <c r="G74">
-        <v>0.03</v>
+        <v>17.94</v>
       </c>
       <c r="H74">
-        <v>17.94</v>
-      </c>
-      <c r="I74">
-        <v>298.6</v>
+        <v>298.58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>